<commit_message>
Major Changes and Customers Completed
</commit_message>
<xml_diff>
--- a/Excel Sheet.xlsx
+++ b/Excel Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaishnavi D\Documents\Projects\Car_Rental_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D460DD-8C60-49B9-95D9-9E7C575C50DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91663A81-86D1-48BE-B28E-F01530293F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{346B649C-0AC4-47A4-A5AB-90B3EBEE42C0}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,7 +751,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>

</xml_diff>